<commit_message>
Updating LCOH & emissions charts for MN fact sheet
</commit_message>
<xml_diff>
--- a/state_fact_sheets/data/modified/lcoh_policy_results.xlsx
+++ b/state_fact_sheets/data/modified/lcoh_policy_results.xlsx
@@ -378,7 +378,8 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Scenario 4 - 100% Cost Share</t>
+          <t>Scenario 4 - 100% Capex
+Share</t>
         </is>
       </c>
     </row>
@@ -390,7 +391,8 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Scenario 4 - 100% Cost Share</t>
+          <t>Scenario 4 - 100% Capex
+Share</t>
         </is>
       </c>
     </row>
@@ -402,7 +404,11 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Scenario 4 - 100% Cost Share, Scenario 4 - 30% Cost Share, Scenario 4 - 50% Cost Share, Scenario 4 - Low Rate, Scenario 4 - No Policy</t>
+          <t>Scenario 4 - 100% Capex
+Share, Scenario 4 - 30% Capex
+Share, Scenario 4 - 50% Capex
+Share, Scenario 4 - Low Elec.
+Rate, Scenario 4 - No Policy</t>
         </is>
       </c>
     </row>
@@ -414,7 +420,11 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Scenario 4 - 100% Cost Share, Scenario 4 - 30% Cost Share, Scenario 4 - 50% Cost Share, Scenario 4 - Low Rate, Scenario 4 - No Policy</t>
+          <t>Scenario 4 - 100% Capex
+Share, Scenario 4 - 30% Capex
+Share, Scenario 4 - 50% Capex
+Share, Scenario 4 - Low Elec.
+Rate, Scenario 4 - No Policy</t>
         </is>
       </c>
     </row>
@@ -426,7 +436,11 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Scenario 4 - 100% Cost Share, Scenario 4 - 30% Cost Share, Scenario 4 - 50% Cost Share, Scenario 4 - Low Rate, Scenario 4 - No Policy</t>
+          <t>Scenario 4 - 100% Capex
+Share, Scenario 4 - 30% Capex
+Share, Scenario 4 - 50% Capex
+Share, Scenario 4 - Low Elec.
+Rate, Scenario 4 - No Policy</t>
         </is>
       </c>
     </row>
@@ -438,7 +452,11 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Scenario 4 - 100% Cost Share, Scenario 4 - 30% Cost Share, Scenario 4 - 50% Cost Share, Scenario 4 - Low Rate, Scenario 4 - No Policy</t>
+          <t>Scenario 4 - 100% Capex
+Share, Scenario 4 - 30% Capex
+Share, Scenario 4 - 50% Capex
+Share, Scenario 4 - Low Elec.
+Rate, Scenario 4 - No Policy</t>
         </is>
       </c>
     </row>
@@ -450,7 +468,11 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Scenario 4 - 100% Cost Share, Scenario 4 - 30% Cost Share, Scenario 4 - 50% Cost Share, Scenario 4 - Low Rate, Scenario 4 - No Policy</t>
+          <t>Scenario 4 - 100% Capex
+Share, Scenario 4 - 30% Capex
+Share, Scenario 4 - 50% Capex
+Share, Scenario 4 - Low Elec.
+Rate, Scenario 4 - No Policy</t>
         </is>
       </c>
     </row>
@@ -462,7 +484,11 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Scenario 4 - 100% Cost Share, Scenario 4 - 30% Cost Share, Scenario 4 - 50% Cost Share, Scenario 4 - Low Rate, Scenario 4 - No Policy</t>
+          <t>Scenario 4 - 100% Capex
+Share, Scenario 4 - 30% Capex
+Share, Scenario 4 - 50% Capex
+Share, Scenario 4 - Low Elec.
+Rate, Scenario 4 - No Policy</t>
         </is>
       </c>
     </row>
@@ -474,7 +500,11 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Scenario 4 - 100% Cost Share, Scenario 4 - 30% Cost Share, Scenario 4 - 50% Cost Share, Scenario 4 - Low Rate, Scenario 4 - No Policy</t>
+          <t>Scenario 4 - 100% Capex
+Share, Scenario 4 - 30% Capex
+Share, Scenario 4 - 50% Capex
+Share, Scenario 4 - Low Elec.
+Rate, Scenario 4 - No Policy</t>
         </is>
       </c>
     </row>
@@ -486,7 +516,11 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Scenario 4 - 100% Cost Share, Scenario 4 - 30% Cost Share, Scenario 4 - 50% Cost Share, Scenario 4 - Low Rate, Scenario 4 - No Policy</t>
+          <t>Scenario 4 - 100% Capex
+Share, Scenario 4 - 30% Capex
+Share, Scenario 4 - 50% Capex
+Share, Scenario 4 - Low Elec.
+Rate, Scenario 4 - No Policy</t>
         </is>
       </c>
     </row>
@@ -498,7 +532,11 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Scenario 4 - 100% Cost Share, Scenario 4 - 30% Cost Share, Scenario 4 - 50% Cost Share, Scenario 4 - Low Rate, Scenario 4 - No Policy</t>
+          <t>Scenario 4 - 100% Capex
+Share, Scenario 4 - 30% Capex
+Share, Scenario 4 - 50% Capex
+Share, Scenario 4 - Low Elec.
+Rate, Scenario 4 - No Policy</t>
         </is>
       </c>
     </row>
@@ -510,7 +548,11 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Scenario 4 - 100% Cost Share, Scenario 4 - 30% Cost Share, Scenario 4 - 50% Cost Share, Scenario 4 - Low Rate, Scenario 4 - No Policy</t>
+          <t>Scenario 4 - 100% Capex
+Share, Scenario 4 - 30% Capex
+Share, Scenario 4 - 50% Capex
+Share, Scenario 4 - Low Elec.
+Rate, Scenario 4 - No Policy</t>
         </is>
       </c>
     </row>
@@ -522,7 +564,11 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Scenario 4 - 100% Cost Share, Scenario 4 - 30% Cost Share, Scenario 4 - 50% Cost Share, Scenario 4 - Low Rate, Scenario 4 - No Policy</t>
+          <t>Scenario 4 - 100% Capex
+Share, Scenario 4 - 30% Capex
+Share, Scenario 4 - 50% Capex
+Share, Scenario 4 - Low Elec.
+Rate, Scenario 4 - No Policy</t>
         </is>
       </c>
     </row>
@@ -534,7 +580,11 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Scenario 4 - 100% Cost Share, Scenario 4 - 30% Cost Share, Scenario 4 - 50% Cost Share, Scenario 4 - Low Rate, Scenario 4 - No Policy</t>
+          <t>Scenario 4 - 100% Capex
+Share, Scenario 4 - 30% Capex
+Share, Scenario 4 - 50% Capex
+Share, Scenario 4 - Low Elec.
+Rate, Scenario 4 - No Policy</t>
         </is>
       </c>
     </row>
@@ -546,7 +596,11 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Scenario 4 - 100% Cost Share, Scenario 4 - 30% Cost Share, Scenario 4 - 50% Cost Share, Scenario 4 - Low Rate, Scenario 4 - No Policy</t>
+          <t>Scenario 4 - 100% Capex
+Share, Scenario 4 - 30% Capex
+Share, Scenario 4 - 50% Capex
+Share, Scenario 4 - Low Elec.
+Rate, Scenario 4 - No Policy</t>
         </is>
       </c>
     </row>
@@ -558,7 +612,11 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Scenario 4 - 100% Cost Share, Scenario 4 - 30% Cost Share, Scenario 4 - 50% Cost Share, Scenario 4 - Low Rate, Scenario 4 - No Policy</t>
+          <t>Scenario 4 - 100% Capex
+Share, Scenario 4 - 30% Capex
+Share, Scenario 4 - 50% Capex
+Share, Scenario 4 - Low Elec.
+Rate, Scenario 4 - No Policy</t>
         </is>
       </c>
     </row>
@@ -570,7 +628,11 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Scenario 4 - 100% Cost Share, Scenario 4 - 30% Cost Share, Scenario 4 - 50% Cost Share, Scenario 4 - Low Rate, Scenario 4 - No Policy</t>
+          <t>Scenario 4 - 100% Capex
+Share, Scenario 4 - 30% Capex
+Share, Scenario 4 - 50% Capex
+Share, Scenario 4 - Low Elec.
+Rate, Scenario 4 - No Policy</t>
         </is>
       </c>
     </row>
@@ -582,7 +644,11 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Scenario 4 - 100% Cost Share, Scenario 4 - 30% Cost Share, Scenario 4 - 50% Cost Share, Scenario 4 - Low Rate, Scenario 4 - No Policy</t>
+          <t>Scenario 4 - 100% Capex
+Share, Scenario 4 - 30% Capex
+Share, Scenario 4 - 50% Capex
+Share, Scenario 4 - Low Elec.
+Rate, Scenario 4 - No Policy</t>
         </is>
       </c>
     </row>
@@ -594,7 +660,11 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Scenario 4 - 100% Cost Share, Scenario 4 - 30% Cost Share, Scenario 4 - 50% Cost Share, Scenario 4 - Low Rate</t>
+          <t>Scenario 4 - 100% Capex
+Share, Scenario 4 - 30% Capex
+Share, Scenario 4 - 50% Capex
+Share, Scenario 4 - Low Elec.
+Rate</t>
         </is>
       </c>
     </row>
@@ -606,7 +676,11 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Scenario 4 - 100% Cost Share, Scenario 4 - 30% Cost Share, Scenario 4 - 50% Cost Share, Scenario 4 - Low Rate, Scenario 4 - No Policy</t>
+          <t>Scenario 4 - 100% Capex
+Share, Scenario 4 - 30% Capex
+Share, Scenario 4 - 50% Capex
+Share, Scenario 4 - Low Elec.
+Rate, Scenario 4 - No Policy</t>
         </is>
       </c>
     </row>
@@ -618,7 +692,8 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Scenario 4 - 100% Cost Share</t>
+          <t>Scenario 4 - 100% Capex
+Share</t>
         </is>
       </c>
     </row>
@@ -642,7 +717,8 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Scenario 4 - 100% Cost Share</t>
+          <t>Scenario 4 - 100% Capex
+Share</t>
         </is>
       </c>
     </row>
@@ -654,7 +730,10 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Scenario 4 - 100% Cost Share, Scenario 4 - 50% Cost Share, Scenario 4 - Low Rate</t>
+          <t>Scenario 4 - 100% Capex
+Share, Scenario 4 - 50% Capex
+Share, Scenario 4 - Low Elec.
+Rate</t>
         </is>
       </c>
     </row>
@@ -679,22 +758,26 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Scenario 4 - 100% Cost Share</t>
+          <t>Scenario 4 - 100% Capex
+Share</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Scenario 4 - 50% Cost Share</t>
+          <t>Scenario 4 - 50% Capex
+Share</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Scenario 4 - Low Rate</t>
+          <t>Scenario 4 - Low Elec.
+Rate</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Scenario 4 - 30% Cost Share</t>
+          <t>Scenario 4 - 30% Capex
+Share</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">

</xml_diff>